<commit_message>
Adicionando as informações sobre idade materna
</commit_message>
<xml_diff>
--- a/f2_tabelas/tabela_resumo_prematuridade.xlsx
+++ b/f2_tabelas/tabela_resumo_prematuridade.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -428,6 +428,21 @@
           <t>Total de partos termo precoce espontâneos (PTPes)</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Média de idade materna</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Idade materna com  &lt;= 15 anos</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Idade materna com  &gt;= 35 anos</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -472,6 +487,15 @@
       <c r="N2">
         <v>25577</v>
       </c>
+      <c r="O2">
+        <v>26.91</v>
+      </c>
+      <c r="P2">
+        <v>10917</v>
+      </c>
+      <c r="Q2">
+        <v>85168</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -516,6 +540,15 @@
       <c r="N3">
         <v>28813</v>
       </c>
+      <c r="O3">
+        <v>27.01</v>
+      </c>
+      <c r="P3">
+        <v>11039</v>
+      </c>
+      <c r="Q3">
+        <v>87050</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -560,6 +593,15 @@
       <c r="N4">
         <v>29909</v>
       </c>
+      <c r="O4">
+        <v>27.16</v>
+      </c>
+      <c r="P4">
+        <v>11209</v>
+      </c>
+      <c r="Q4">
+        <v>94104</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -604,6 +646,15 @@
       <c r="N5">
         <v>30405</v>
       </c>
+      <c r="O5">
+        <v>27.34</v>
+      </c>
+      <c r="P5">
+        <v>10343</v>
+      </c>
+      <c r="Q5">
+        <v>99964</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -648,6 +699,15 @@
       <c r="N6">
         <v>32880</v>
       </c>
+      <c r="O6">
+        <v>27.49</v>
+      </c>
+      <c r="P6">
+        <v>8859</v>
+      </c>
+      <c r="Q6">
+        <v>99693</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -692,6 +752,15 @@
       <c r="N7">
         <v>33517</v>
       </c>
+      <c r="O7">
+        <v>27.77</v>
+      </c>
+      <c r="P7">
+        <v>7909</v>
+      </c>
+      <c r="Q7">
+        <v>109014</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -736,6 +805,15 @@
       <c r="N8">
         <v>33585</v>
       </c>
+      <c r="O8">
+        <v>28.03</v>
+      </c>
+      <c r="P8">
+        <v>7093</v>
+      </c>
+      <c r="Q8">
+        <v>115692</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -780,6 +858,15 @@
       <c r="N9">
         <v>32791</v>
       </c>
+      <c r="O9">
+        <v>28.19</v>
+      </c>
+      <c r="P9">
+        <v>6207</v>
+      </c>
+      <c r="Q9">
+        <v>115337</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -824,6 +911,15 @@
       <c r="N10">
         <v>29643</v>
       </c>
+      <c r="O10">
+        <v>28.27</v>
+      </c>
+      <c r="P10">
+        <v>5574</v>
+      </c>
+      <c r="Q10">
+        <v>110781</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -868,6 +964,15 @@
       <c r="N11">
         <v>27112</v>
       </c>
+      <c r="O11">
+        <v>28.37</v>
+      </c>
+      <c r="P11">
+        <v>5138</v>
+      </c>
+      <c r="Q11">
+        <v>107904</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -912,6 +1017,15 @@
       <c r="N12">
         <v>27344</v>
       </c>
+      <c r="O12">
+        <v>28.59</v>
+      </c>
+      <c r="P12">
+        <v>4189</v>
+      </c>
+      <c r="Q12">
+        <v>109063</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -955,6 +1069,15 @@
       </c>
       <c r="N13">
         <v>28483</v>
+      </c>
+      <c r="O13">
+        <v>28.62</v>
+      </c>
+      <c r="P13">
+        <v>3944</v>
+      </c>
+      <c r="Q13">
+        <v>107376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>